<commit_message>
Added small and large values
</commit_message>
<xml_diff>
--- a/AtmosphericDensity.xlsx
+++ b/AtmosphericDensity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwapman/Documents/SmallSatSeparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3D5CD1-84FA-3041-AFB7-4B0F359B85FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED34F47A-DFCE-484A-80A0-BB714FCE2FB7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16700" xr2:uid="{FA41E5A0-8A03-CD4E-8870-9A2519EF4FFE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16680" xr2:uid="{FA41E5A0-8A03-CD4E-8870-9A2519EF4FFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>h</t>
+    <t>h (km)</t>
   </si>
   <si>
-    <t>rhoMin</t>
+    <t>rhoMin (g/km3)</t>
   </si>
   <si>
-    <t>rhoMax</t>
+    <t>rhoMax (g/km3)</t>
   </si>
   <si>
-    <t>93..08</t>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Inf altitude</t>
   </si>
 </sst>
 </file>
@@ -72,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,15 +395,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBA1830-36B0-1D4D-B984-93A5E0B81DAB}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,555 +418,586 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1225000000000</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1225000000000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>100</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>497400</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>497400</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>120</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>24900</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>24900</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>130</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>8377</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>8710</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>140</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>3899</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>4059</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>150</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2122</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>2215</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>160</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>1263</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>1344</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>170</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>800.8</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>875.8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>180</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>528.29999999999995</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>601</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>190</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>361.7</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>429.7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>200</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>255.7</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>316.2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>210</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>183.9</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>239.6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>220</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>134.1</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>185.3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>230</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>99.49</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>145.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>240</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>74.88</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>115.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>250</v>
-      </c>
-      <c r="B16">
-        <v>57.09</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B17">
-        <v>44.03</v>
+        <v>57.09</v>
       </c>
       <c r="C17">
-        <v>75.55</v>
+        <v>93.08</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B18">
-        <v>34.299999999999997</v>
+        <v>44.03</v>
       </c>
       <c r="C18">
-        <v>61.82</v>
+        <v>75.55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B19">
-        <v>26.97</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="C19">
-        <v>50.95</v>
+        <v>61.82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B20">
-        <v>21.39</v>
+        <v>26.97</v>
       </c>
       <c r="C20">
-        <v>42.26</v>
+        <v>50.95</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B21">
-        <v>17.079999999999998</v>
+        <v>21.39</v>
       </c>
       <c r="C21">
-        <v>35.26</v>
+        <v>42.26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="B22">
-        <v>10.99</v>
+        <v>17.079999999999998</v>
       </c>
       <c r="C22">
-        <v>25.11</v>
+        <v>35.26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="B23">
-        <v>7.2140000000000004</v>
+        <v>10.99</v>
       </c>
       <c r="C23">
-        <v>18.190000000000001</v>
+        <v>25.11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="B24">
-        <v>4.8239999999999998</v>
+        <v>7.2140000000000004</v>
       </c>
       <c r="C24">
-        <v>13.37</v>
+        <v>18.190000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="B25">
-        <v>3.274</v>
+        <v>4.8239999999999998</v>
       </c>
       <c r="C25">
-        <v>9.9550000000000001</v>
+        <v>13.37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="B26">
-        <v>2.2490000000000001</v>
+        <v>3.274</v>
       </c>
       <c r="C26">
-        <v>7.492</v>
+        <v>9.9550000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="B27">
-        <v>1.5580000000000001</v>
+        <v>2.2490000000000001</v>
       </c>
       <c r="C27">
-        <v>5.6840000000000002</v>
+        <v>7.492</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="B28">
-        <v>1.091</v>
+        <v>1.5580000000000001</v>
       </c>
       <c r="C28">
-        <v>4.3550000000000004</v>
+        <v>5.6840000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="B29">
-        <v>0.77010000000000001</v>
+        <v>1.091</v>
       </c>
       <c r="C29">
-        <v>3.3620000000000001</v>
+        <v>4.3550000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="B30">
-        <v>0.5474</v>
+        <v>0.77010000000000001</v>
       </c>
       <c r="C30">
-        <v>2.6120000000000001</v>
+        <v>3.3620000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="B31">
-        <v>0.3916</v>
+        <v>0.5474</v>
       </c>
       <c r="C31">
-        <v>2.0419999999999998</v>
+        <v>2.6120000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="B32">
-        <v>0.28189999999999998</v>
+        <v>0.3916</v>
       </c>
       <c r="C32">
-        <v>1.605</v>
+        <v>2.0419999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="B33">
-        <v>0.20419999999999999</v>
+        <v>0.28189999999999998</v>
       </c>
       <c r="C33">
-        <v>1.2669999999999999</v>
+        <v>1.605</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="B34">
-        <v>0.14879999999999999</v>
+        <v>0.20419999999999999</v>
       </c>
       <c r="C34">
-        <v>1.0049999999999999</v>
+        <v>1.2669999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="B35">
-        <v>0.10920000000000001</v>
+        <v>0.14879999999999999</v>
       </c>
       <c r="C35">
-        <v>0.79969999999999997</v>
+        <v>1.0049999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="B36">
-        <v>8.0699999999999994E-2</v>
+        <v>0.10920000000000001</v>
       </c>
       <c r="C36">
-        <v>0.63900000000000001</v>
+        <v>0.79969999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="B37">
-        <v>6.012E-2</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="C37">
-        <v>0.51229999999999998</v>
+        <v>0.63900000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>640</v>
+        <v>620</v>
       </c>
       <c r="B38">
-        <v>4.5190000000000001E-2</v>
+        <v>6.012E-2</v>
       </c>
       <c r="C38">
-        <v>0.41210000000000002</v>
+        <v>0.51229999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>660</v>
+        <v>640</v>
       </c>
       <c r="B39">
-        <v>3.4299999999999997E-2</v>
+        <v>4.5190000000000001E-2</v>
       </c>
       <c r="C39">
-        <v>0.33250000000000002</v>
+        <v>0.41210000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>680</v>
+        <v>660</v>
       </c>
       <c r="B40">
-        <v>2.632E-2</v>
+        <v>3.4299999999999997E-2</v>
       </c>
       <c r="C40">
-        <v>0.26910000000000001</v>
+        <v>0.33250000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>700</v>
+        <v>680</v>
       </c>
       <c r="B41">
-        <v>2.043E-2</v>
+        <v>2.632E-2</v>
       </c>
       <c r="C41">
-        <v>0.2185</v>
+        <v>0.26910000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>720</v>
+        <v>700</v>
       </c>
       <c r="B42">
-        <v>1.6070000000000001E-2</v>
+        <v>2.043E-2</v>
       </c>
       <c r="C42">
-        <v>0.1779</v>
+        <v>0.2185</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>740</v>
+        <v>720</v>
       </c>
       <c r="B43">
-        <v>1.281E-2</v>
+        <v>1.6070000000000001E-2</v>
       </c>
       <c r="C43">
-        <v>0.1452</v>
+        <v>0.1779</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>760</v>
+        <v>740</v>
       </c>
       <c r="B44">
-        <v>1.0359999999999999E-2</v>
+        <v>1.281E-2</v>
       </c>
       <c r="C44">
-        <v>0.11899999999999999</v>
+        <v>0.1452</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>780</v>
+        <v>760</v>
       </c>
       <c r="B45">
-        <v>8.4960000000000001E-3</v>
+        <v>1.0359999999999999E-2</v>
       </c>
       <c r="C45">
-        <v>9.776E-2</v>
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>800</v>
+        <v>780</v>
       </c>
       <c r="B46">
-        <v>7.0689999999999998E-3</v>
+        <v>8.4960000000000001E-3</v>
       </c>
       <c r="C46">
-        <v>8.0589999999999995E-2</v>
+        <v>9.776E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>840</v>
+        <v>800</v>
       </c>
       <c r="B47">
-        <v>4.6800000000000001E-3</v>
+        <v>7.0689999999999998E-3</v>
       </c>
       <c r="C47">
-        <v>5.7410000000000003E-2</v>
+        <v>8.0589999999999995E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
+        <v>840</v>
+      </c>
+      <c r="B48">
+        <v>4.6800000000000001E-3</v>
+      </c>
+      <c r="C48">
+        <v>5.7410000000000003E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
         <v>880</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>4.2099999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
         <v>920</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>2.2100000000000002E-3</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>3.1300000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
         <v>960</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>1.56E-3</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
         <v>1000</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>1.15E-3</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <v>1.8100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>10000000000</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>